<commit_message>
Update Journal de bord CPNVoiturage.xlsx
</commit_message>
<xml_diff>
--- a/Documents/Journal de bord CPNVoiturage.xlsx
+++ b/Documents/Journal de bord CPNVoiturage.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -95,9 +95,6 @@
     <t>Fond, Accueil, Nouveau compte, Vue</t>
   </si>
   <si>
-    <t>Début du MCD</t>
-  </si>
-  <si>
     <t>Entrevue pour le premier sprint</t>
   </si>
   <si>
@@ -105,6 +102,24 @@
   </si>
   <si>
     <t>Refonte et mise au propre du MCD</t>
+  </si>
+  <si>
+    <t>Début du MCD-MLD</t>
+  </si>
+  <si>
+    <t>Premiers dessins de MLD</t>
+  </si>
+  <si>
+    <t>Dessins rapides d'un modèle de MLD</t>
+  </si>
+  <si>
+    <t>Refonte et mise au propre du MLD</t>
+  </si>
+  <si>
+    <t>Ajout de la notion d'horaire au MCD et MLD</t>
+  </si>
+  <si>
+    <t>Gestion des periodes d'arrivées et de départ, des villes et de EDT</t>
   </si>
 </sst>
 </file>
@@ -498,8 +513,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="C2:F85" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
-  <autoFilter ref="C2:F85"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="C2:F87" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
+  <autoFilter ref="C2:F87"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Tâche" dataDxfId="3"/>
     <tableColumn id="3" name="Date" dataDxfId="2"/>
@@ -776,17 +791,17 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:F86"/>
+  <dimension ref="B1:F88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.140625" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="34.42578125" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
     <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" customWidth="1"/>
     <col min="6" max="6" width="91.5703125" customWidth="1"/>
@@ -878,76 +893,78 @@
         <v>44229</v>
       </c>
       <c r="E7" s="14">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="F7" s="15" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="C8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="10">
+        <v>44229</v>
+      </c>
+      <c r="E8" s="11">
+        <v>25</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D9" s="12">
         <v>44231</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E9" s="11">
         <v>65</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="10">
-        <v>44231</v>
-      </c>
-      <c r="E9" s="11">
-        <v>60</v>
-      </c>
-      <c r="F9" s="5"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C10" s="9" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D10" s="10">
         <v>44231</v>
       </c>
       <c r="E10" s="11">
-        <v>90</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F10" s="5"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C11" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D11" s="10">
         <v>44231</v>
       </c>
       <c r="E11" s="11">
-        <v>45</v>
-      </c>
-      <c r="F11" s="5"/>
+        <v>90</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C12" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D12" s="10">
-        <v>44232</v>
+        <v>44231</v>
       </c>
       <c r="E12" s="11">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="F12" s="5"/>
     </row>
@@ -959,51 +976,71 @@
         <v>44232</v>
       </c>
       <c r="E13" s="11">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C14" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D14" s="10">
         <v>44232</v>
       </c>
       <c r="E14" s="11">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C15" s="9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D15" s="10">
         <v>44232</v>
       </c>
       <c r="E15" s="11">
+        <v>30</v>
+      </c>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C16" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="10">
+        <v>44232</v>
+      </c>
+      <c r="E16" s="11">
+        <v>20</v>
+      </c>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C17" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="10">
+        <v>44232</v>
+      </c>
+      <c r="E17" s="11">
+        <v>25</v>
+      </c>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C18" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="10">
+        <v>44235</v>
+      </c>
+      <c r="E18" s="11">
         <v>45</v>
       </c>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C16" s="9"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C17" s="9"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="5"/>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C18" s="9"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="5"/>
+      <c r="F18" s="5" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" s="9"/>
@@ -1401,11 +1438,23 @@
       <c r="E84" s="11"/>
       <c r="F84" s="5"/>
     </row>
+    <row r="85" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C85" s="9"/>
+      <c r="D85" s="10"/>
+      <c r="E85" s="11"/>
+      <c r="F85" s="5"/>
+    </row>
     <row r="86" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C86" s="16"/>
-      <c r="D86" s="17"/>
-      <c r="E86" s="18"/>
-      <c r="F86" s="19"/>
+      <c r="C86" s="9"/>
+      <c r="D86" s="10"/>
+      <c r="E86" s="11"/>
+      <c r="F86" s="5"/>
+    </row>
+    <row r="88" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C88" s="16"/>
+      <c r="D88" s="17"/>
+      <c r="E88" s="18"/>
+      <c r="F88" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ajout de css responsive pour les onglets
</commit_message>
<xml_diff>
--- a/Documents/Journal de bord CPNVoiturage.xlsx
+++ b/Documents/Journal de bord CPNVoiturage.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>Date</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t>Création de la structure de la page avec la gestion des onglets et le css</t>
+  </si>
+  <si>
+    <t>Tests de CSS</t>
+  </si>
+  <si>
+    <t>Tests de css pour des onglets responsive</t>
   </si>
 </sst>
 </file>
@@ -841,8 +847,8 @@
   </sheetPr>
   <dimension ref="B1:F89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="E19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1203,10 +1209,18 @@
       </c>
     </row>
     <row r="27" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C27" s="9"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="5"/>
+      <c r="C27" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="10">
+        <v>44242</v>
+      </c>
+      <c r="E27" s="11">
+        <v>100</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="28" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C28" s="9"/>

</xml_diff>

<commit_message>
Mise à jour du JdB et de la planif
</commit_message>
<xml_diff>
--- a/Documents/Journal de bord CPNVoiturage.xlsx
+++ b/Documents/Journal de bord CPNVoiturage.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
   <si>
     <t>Date</t>
   </si>
@@ -173,7 +173,31 @@
     <t>Tests de CSS</t>
   </si>
   <si>
-    <t>Tests de css pour des onglets responsive</t>
+    <t>Tests de css pour avoir des onglets responsive</t>
+  </si>
+  <si>
+    <t>Implémentation complète du gabarit</t>
+  </si>
+  <si>
+    <t>Connecter le gabarit correctement et ajout correct de la vue au choix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Création </t>
+  </si>
+  <si>
+    <t>Création et gestion du css de la page du profil</t>
+  </si>
+  <si>
+    <t>Javascript pour disable tous les champs désactivés en fonction des jours</t>
+  </si>
+  <si>
+    <t>JS pour les choxi des jours</t>
+  </si>
+  <si>
+    <t>Création de la page de login et du css</t>
+  </si>
+  <si>
+    <t>Création de la page de login</t>
   </si>
 </sst>
 </file>
@@ -847,8 +871,8 @@
   </sheetPr>
   <dimension ref="B1:F89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1223,28 +1247,60 @@
       </c>
     </row>
     <row r="28" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C28" s="9"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="5"/>
+      <c r="C28" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="10">
+        <v>44245</v>
+      </c>
+      <c r="E28" s="11">
+        <v>100</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="29" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C29" s="9"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="5"/>
+      <c r="C29" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="10">
+        <v>44245</v>
+      </c>
+      <c r="E29" s="11">
+        <v>100</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="30" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C30" s="9"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="5"/>
+      <c r="C30" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="10">
+        <v>44245</v>
+      </c>
+      <c r="E30" s="11">
+        <v>45</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="31" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C31" s="9"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="5"/>
+      <c r="C31" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="10">
+        <v>44246</v>
+      </c>
+      <c r="E31" s="11">
+        <v>100</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="32" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C32" s="9"/>

</xml_diff>

<commit_message>
Mise à jour de la doc et documents
</commit_message>
<xml_diff>
--- a/Documents/Journal de bord CPNVoiturage.xlsx
+++ b/Documents/Journal de bord CPNVoiturage.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="1185" windowWidth="21675" windowHeight="10920"/>
+    <workbookView xWindow="4440" yWindow="1185" windowWidth="7785" windowHeight="5565"/>
   </bookViews>
   <sheets>
     <sheet name="Page 1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
   <si>
     <t>Date</t>
   </si>
@@ -198,6 +198,55 @@
   </si>
   <si>
     <t>Création de la page de login</t>
+  </si>
+  <si>
+    <t>Gestion des liens entre les pages</t>
+  </si>
+  <si>
+    <t>Affichage dynamique des voitures</t>
+  </si>
+  <si>
+    <t>Définition des variables à utiliser pour 
+l'affichage dynamique</t>
+  </si>
+  <si>
+    <t>Gestion des jours et du profil, de façon uniforme</t>
+  </si>
+  <si>
+    <t>Stockages de toutes les données dans des tableaux multidimensionnels</t>
+  </si>
+  <si>
+    <t>Affichage dynamique des tableaux</t>
+  </si>
+  <si>
+    <t>Affichage dynamique des places restantes et des couleurs de lignes</t>
+  </si>
+  <si>
+    <t>Finir l'affichage dynamique des voitures</t>
+  </si>
+  <si>
+    <t>Affichage dynamique du profil</t>
+  </si>
+  <si>
+    <t>Affichage d'un jour de façon dynamique</t>
+  </si>
+  <si>
+    <t>Automatisme des jours de la semaine</t>
+  </si>
+  <si>
+    <t>Gestion d'un tableau pour afficher tous les jours avec une boucle</t>
+  </si>
+  <si>
+    <t>Retouche du css</t>
+  </si>
+  <si>
+    <t>Enlever les couleurs de debug et mise à niveau de la responsivité</t>
+  </si>
+  <si>
+    <t>Création de la base de donnée</t>
+  </si>
+  <si>
+    <t>Création de la DB</t>
   </si>
 </sst>
 </file>
@@ -403,7 +452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
@@ -455,6 +504,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -871,8 +923,8 @@
   </sheetPr>
   <dimension ref="B1:F89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1303,52 +1355,116 @@
       </c>
     </row>
     <row r="32" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C32" s="9"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="5"/>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C33" s="9"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="5"/>
+      <c r="C32" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D32" s="10">
+        <v>44256</v>
+      </c>
+      <c r="E32" s="11">
+        <v>30</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C33" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D33" s="10">
+        <v>44256</v>
+      </c>
+      <c r="E33" s="11">
+        <v>45</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C34" s="9"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="5"/>
+      <c r="C34" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" s="10">
+        <v>44256</v>
+      </c>
+      <c r="E34" s="11">
+        <v>45</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C35" s="9"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="5"/>
+      <c r="C35" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" s="10">
+        <v>44258</v>
+      </c>
+      <c r="E35" s="11">
+        <v>30</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C36" s="9"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="5"/>
+      <c r="C36" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" s="10">
+        <v>44259</v>
+      </c>
+      <c r="E36" s="11">
+        <v>45</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="37" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C37" s="9"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="5"/>
+      <c r="C37" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D37" s="10">
+        <v>44259</v>
+      </c>
+      <c r="E37" s="11">
+        <v>80</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="38" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C38" s="9"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="5"/>
+      <c r="C38" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38" s="10">
+        <v>44259</v>
+      </c>
+      <c r="E38" s="11">
+        <v>30</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="39" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C39" s="9"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="5"/>
+      <c r="C39" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D39" s="10">
+        <v>44259</v>
+      </c>
+      <c r="E39" s="11">
+        <v>120</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="40" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C40" s="9"/>

</xml_diff>

<commit_message>
Actualisation de la doc
</commit_message>
<xml_diff>
--- a/Documents/Journal de bord CPNVoiturage.xlsx
+++ b/Documents/Journal de bord CPNVoiturage.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="90">
   <si>
     <t>Date</t>
   </si>
@@ -247,6 +247,60 @@
   </si>
   <si>
     <t>Création de la DB</t>
+  </si>
+  <si>
+    <t>Remplissage de la base de données</t>
+  </si>
+  <si>
+    <t>Ajout de données de test</t>
+  </si>
+  <si>
+    <t>Sprint 1 review + site en ligne</t>
+  </si>
+  <si>
+    <t>Accès au site en ligne (mycpnv) et cloture du sprint 2</t>
+  </si>
+  <si>
+    <t>Création du DB connetor</t>
+  </si>
+  <si>
+    <t>Tests avec la connexion à la DB et des fonctions de requêtes select et insert</t>
+  </si>
+  <si>
+    <t>Affichage des villes sur les register</t>
+  </si>
+  <si>
+    <t>Gestion du formulaire de register</t>
+  </si>
+  <si>
+    <t>Formulaire HTML et vérification des données coté PHP</t>
+  </si>
+  <si>
+    <t>Requête et hash du password</t>
+  </si>
+  <si>
+    <t>Gestion du formulaire de login</t>
+  </si>
+  <si>
+    <t>Requêtes du register</t>
+  </si>
+  <si>
+    <t>Requêtes du login</t>
+  </si>
+  <si>
+    <t>Requête et password verify</t>
+  </si>
+  <si>
+    <t>Création de la requête pour l'affichage des voitures</t>
+  </si>
+  <si>
+    <t>Création d'une requête unique pour afficher toutes les voitures du jour</t>
+  </si>
+  <si>
+    <t>Sécurisation et gestion des erreurs du login</t>
+  </si>
+  <si>
+    <t>Affichage des erreurs et réaffichage des données envoyées en cas d'erreur</t>
   </si>
 </sst>
 </file>
@@ -452,7 +506,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
@@ -508,6 +562,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -643,8 +700,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="C2:F88" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
-  <autoFilter ref="C2:F88"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="C2:F90" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
+  <autoFilter ref="C2:F90"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Tâche" dataDxfId="3"/>
     <tableColumn id="3" name="Date" dataDxfId="2"/>
@@ -921,10 +978,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:F89"/>
+  <dimension ref="B1:F91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="C40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1467,64 +1524,142 @@
       </c>
     </row>
     <row r="40" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C40" s="9"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="5"/>
+      <c r="C40" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D40" s="10">
+        <v>44263</v>
+      </c>
+      <c r="E40" s="11">
+        <v>60</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="41" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C41" s="9"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="5"/>
+      <c r="C41" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D41" s="10">
+        <v>44263</v>
+      </c>
+      <c r="E41" s="11">
+        <v>80</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="42" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C42" s="9"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="5"/>
+      <c r="C42" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D42" s="10">
+        <v>44266</v>
+      </c>
+      <c r="E42" s="11">
+        <v>60</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="43" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C43" s="9"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="11"/>
+      <c r="C43" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D43" s="10">
+        <v>44266</v>
+      </c>
+      <c r="E43" s="11">
+        <v>15</v>
+      </c>
       <c r="F43" s="5"/>
     </row>
     <row r="44" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C44" s="9"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="5"/>
+      <c r="C44" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D44" s="10">
+        <v>44266</v>
+      </c>
+      <c r="E44" s="11">
+        <v>30</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="45" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C45" s="9"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="5"/>
+      <c r="C45" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D45" s="10">
+        <v>44266</v>
+      </c>
+      <c r="E45" s="11">
+        <v>30</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="46" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C46" s="9"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="5"/>
+      <c r="C46" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D46" s="10">
+        <v>44266</v>
+      </c>
+      <c r="E46" s="11">
+        <v>20</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="47" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C47" s="9"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="5"/>
+      <c r="C47" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D47" s="10">
+        <v>44266</v>
+      </c>
+      <c r="E47" s="11">
+        <v>20</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="48" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C48" s="9"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="5"/>
+      <c r="C48" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D48" s="10">
+        <v>44267</v>
+      </c>
+      <c r="E48" s="11">
+        <v>30</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="49" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C49" s="9"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="5"/>
+      <c r="C49" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D49" s="10">
+        <v>44267</v>
+      </c>
+      <c r="E49" s="11">
+        <v>60</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="50" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C50" s="9"/>
@@ -1754,11 +1889,26 @@
       <c r="E87" s="11"/>
       <c r="F87" s="5"/>
     </row>
+    <row r="88" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C88" s="9"/>
+      <c r="D88" s="10"/>
+      <c r="E88" s="11"/>
+      <c r="F88" s="5"/>
+    </row>
     <row r="89" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C89" s="16"/>
-      <c r="D89" s="17"/>
-      <c r="E89" s="18"/>
-      <c r="F89" s="19"/>
+      <c r="C89" s="9"/>
+      <c r="D89" s="10"/>
+      <c r="E89" s="11"/>
+      <c r="F89" s="5"/>
+    </row>
+    <row r="90" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E90" s="21"/>
+    </row>
+    <row r="91" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C91" s="16"/>
+      <c r="D91" s="17"/>
+      <c r="E91" s="18"/>
+      <c r="F91" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Mise à jour de la doc
</commit_message>
<xml_diff>
--- a/Documents/Journal de bord CPNVoiturage.xlsx
+++ b/Documents/Journal de bord CPNVoiturage.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="102">
   <si>
     <t>Date</t>
   </si>
@@ -301,6 +301,42 @@
   </si>
   <si>
     <t>Affichage des erreurs et réaffichage des données envoyées en cas d'erreur</t>
+  </si>
+  <si>
+    <t>Affichage dynamique des données sur le profil</t>
+  </si>
+  <si>
+    <t>Requetes et création du tableau pour l'affichage du profil</t>
+  </si>
+  <si>
+    <t>Utilisation des Ids des périodes pour le profil</t>
+  </si>
+  <si>
+    <t>Gestion des colonnes nécessaires de csv de EDT</t>
+  </si>
+  <si>
+    <t>Affichage de la page admin</t>
+  </si>
+  <si>
+    <t>Récuperation et processing du csv</t>
+  </si>
+  <si>
+    <t>Récuperation pour préparer la requête de EDT</t>
+  </si>
+  <si>
+    <t>Fin de l'importation de EDT</t>
+  </si>
+  <si>
+    <t>Corrections sur le login</t>
+  </si>
+  <si>
+    <t>3 caractères max (coté client et serveur) pour l'acronyme et ajout du signout</t>
+  </si>
+  <si>
+    <t>Refonte d'une requête</t>
+  </si>
+  <si>
+    <t>Refonte de la requête pour afficher les voitures car il manquait certaines personnes seules</t>
   </si>
 </sst>
 </file>
@@ -980,8 +1016,8 @@
   </sheetPr>
   <dimension ref="B1:F91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" topLeftCell="D40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1662,64 +1698,128 @@
       </c>
     </row>
     <row r="50" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C50" s="9"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="11"/>
+      <c r="C50" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D50" s="10">
+        <v>44270</v>
+      </c>
+      <c r="E50" s="11">
+        <v>60</v>
+      </c>
       <c r="F50" s="5"/>
     </row>
     <row r="51" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C51" s="9"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="11"/>
+      <c r="C51" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D51" s="10">
+        <v>44270</v>
+      </c>
+      <c r="E51" s="11">
+        <v>60</v>
+      </c>
       <c r="F51" s="5"/>
     </row>
     <row r="52" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C52" s="9"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="11"/>
+      <c r="C52" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D52" s="10">
+        <v>44273</v>
+      </c>
+      <c r="E52" s="11">
+        <v>45</v>
+      </c>
       <c r="F52" s="5"/>
     </row>
     <row r="53" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C53" s="9"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="11"/>
+      <c r="C53" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D53" s="10">
+        <v>44273</v>
+      </c>
+      <c r="E53" s="11">
+        <v>45</v>
+      </c>
       <c r="F53" s="5"/>
     </row>
     <row r="54" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C54" s="9"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="11"/>
+      <c r="C54" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D54" s="10">
+        <v>44273</v>
+      </c>
+      <c r="E54" s="11">
+        <v>30</v>
+      </c>
       <c r="F54" s="5"/>
     </row>
     <row r="55" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C55" s="9"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="11"/>
+      <c r="C55" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D55" s="10">
+        <v>44273</v>
+      </c>
+      <c r="E55" s="11">
+        <v>80</v>
+      </c>
       <c r="F55" s="5"/>
     </row>
     <row r="56" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C56" s="9"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="11"/>
+      <c r="C56" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D56" s="10">
+        <v>44273</v>
+      </c>
+      <c r="E56" s="11">
+        <v>45</v>
+      </c>
       <c r="F56" s="5"/>
     </row>
     <row r="57" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C57" s="9"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="11"/>
+      <c r="C57" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D57" s="10">
+        <v>44274</v>
+      </c>
+      <c r="E57" s="11">
+        <v>40</v>
+      </c>
       <c r="F57" s="5"/>
     </row>
     <row r="58" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C58" s="9"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="11"/>
-      <c r="F58" s="5"/>
+      <c r="C58" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D58" s="10">
+        <v>44274</v>
+      </c>
+      <c r="E58" s="11">
+        <v>15</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="59" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C59" s="9"/>
-      <c r="D59" s="10"/>
-      <c r="E59" s="11"/>
-      <c r="F59" s="5"/>
+      <c r="C59" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D59" s="10">
+        <v>44274</v>
+      </c>
+      <c r="E59" s="11">
+        <v>70</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="60" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C60" s="9"/>

</xml_diff>

<commit_message>
Doc mise à jour
</commit_message>
<xml_diff>
--- a/Documents/Journal de bord CPNVoiturage.xlsx
+++ b/Documents/Journal de bord CPNVoiturage.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="107">
   <si>
     <t>Date</t>
   </si>
@@ -337,6 +337,21 @@
   </si>
   <si>
     <t>Refonte de la requête pour afficher les voitures car il manquait certaines personnes seules</t>
+  </si>
+  <si>
+    <t>Corrections des requêtes pour afficher les voitures</t>
+  </si>
+  <si>
+    <t>Correction d'un problème de requête qui donnait des doublons pour les conducteurs</t>
+  </si>
+  <si>
+    <t>Changement du menu si l'on est déjà conducteur</t>
+  </si>
+  <si>
+    <t>Affichage si l'on est conducteur ou si l'on est déjà dans une voiture</t>
+  </si>
+  <si>
+    <t>Fonction pour rejoindre une voiture</t>
   </si>
 </sst>
 </file>
@@ -1016,8 +1031,8 @@
   </sheetPr>
   <dimension ref="B1:F91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1822,21 +1837,43 @@
       </c>
     </row>
     <row r="60" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C60" s="9"/>
-      <c r="D60" s="10"/>
-      <c r="E60" s="11"/>
-      <c r="F60" s="5"/>
+      <c r="C60" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D60" s="10">
+        <v>44277</v>
+      </c>
+      <c r="E60" s="11">
+        <v>90</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="61" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C61" s="9"/>
-      <c r="D61" s="10"/>
-      <c r="E61" s="11"/>
-      <c r="F61" s="5"/>
+      <c r="C61" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D61" s="10">
+        <v>44277</v>
+      </c>
+      <c r="E61" s="11">
+        <v>45</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="62" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C62" s="9"/>
-      <c r="D62" s="10"/>
-      <c r="E62" s="11"/>
+      <c r="C62" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D62" s="10">
+        <v>44277</v>
+      </c>
+      <c r="E62" s="11">
+        <v>45</v>
+      </c>
       <c r="F62" s="5"/>
     </row>
     <row r="63" spans="3:6" x14ac:dyDescent="0.25">

</xml_diff>